<commit_message>
Supressed HTML for git language detection
</commit_message>
<xml_diff>
--- a/inst/extdata/Lab_results_new.xlsx
+++ b/inst/extdata/Lab_results_new.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA6F3B4-479D-4B72-B05B-EA4FE0D3B125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259C36D5-CB82-4323-91F0-9ECBBDFF9C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lab_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>notes</t>
   </si>
@@ -177,6 +190,48 @@
   </si>
   <si>
     <t>LS0070-SCV2-PCR</t>
+  </si>
+  <si>
+    <t>Lab B</t>
+  </si>
+  <si>
+    <t>Aminonga</t>
+  </si>
+  <si>
+    <t>Newbie</t>
+  </si>
+  <si>
+    <t>NID200098</t>
+  </si>
+  <si>
+    <t>LS0075-SCV2-PCR</t>
+  </si>
+  <si>
+    <t>Jarat</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>NID200099</t>
+  </si>
+  <si>
+    <t>LS0076-SCV2-PCR</t>
+  </si>
+  <si>
+    <t>Nkindle</t>
+  </si>
+  <si>
+    <t>Newperson</t>
+  </si>
+  <si>
+    <t>NID200100</t>
+  </si>
+  <si>
+    <t>LS0077-SCV2-PCR</t>
+  </si>
+  <si>
+    <t>New case not yet notified</t>
   </si>
 </sst>
 </file>
@@ -184,7 +239,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -226,10 +281,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -577,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -988,6 +1043,174 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3">
+        <v>38671</v>
+      </c>
+      <c r="E8" s="5">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="3">
+        <v>44824</v>
+      </c>
+      <c r="I8" s="3">
+        <v>44825</v>
+      </c>
+      <c r="J8" s="3">
+        <v>44825</v>
+      </c>
+      <c r="K8" s="3">
+        <v>44825</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="5">
+        <v>30.1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>6</v>
+      </c>
+      <c r="R8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3">
+        <v>35866</v>
+      </c>
+      <c r="E9" s="5">
+        <v>24</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="3">
+        <v>44825</v>
+      </c>
+      <c r="I9" s="3">
+        <v>44826</v>
+      </c>
+      <c r="J9" s="3">
+        <v>44826</v>
+      </c>
+      <c r="K9" s="3">
+        <v>44826</v>
+      </c>
+      <c r="L9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="5">
+        <v>25.6</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="3">
+        <v>33109</v>
+      </c>
+      <c r="E10" s="5">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="3">
+        <v>44824</v>
+      </c>
+      <c r="I10" s="3">
+        <v>44825</v>
+      </c>
+      <c r="J10" s="3">
+        <v>44825</v>
+      </c>
+      <c r="K10" s="3">
+        <v>44825</v>
+      </c>
+      <c r="L10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="5">
+        <v>28.4</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>